<commit_message>
- Korrigert spørsmålstekst i malfiler - La til filter for kandidatar der det har gått over tre år sidan dei fullførte, for å sikre godt samanlikningsgrunnlag - Flytta og retta opp feil i oppretting av brutto_arslonn_vasket
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_serie_vars.xlsx
+++ b/malfiler/Kandidat_2022_serie_vars.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/datafiler/kandidat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23F82529-522F-408C-8603-3908B6F67CCD}"/>
+  <xr:revisionPtr revIDLastSave="563" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1E6BC7F-1DB6-4616-ADD1-94E4C2CC2F19}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>dager_til_jobb</t>
   </si>
   <si>
-    <t xml:space="preserve">Hvor lang tid tok det fra du fullførte masterutdanningen til du fikk tilbud om relevant jobb? </t>
-  </si>
-  <si>
     <t>Dager til jobb</t>
   </si>
   <si>
@@ -389,6 +386,9 @@
   </si>
   <si>
     <t>snitt_as_num_serie</t>
+  </si>
+  <si>
+    <t>Hvor lang tid tok det fra du fullførte utdanningen til du fikk tilbud om relevant jobb?</t>
   </si>
 </sst>
 </file>
@@ -600,9 +600,9 @@
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{160CC1CB-F893-4D31-B90C-FCC9EC624563}" name="Spørsmålstekst" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{26B093AC-730D-4DC7-8FEB-A32629DB4F75}" name="Variabel" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{B339D8CC-5E13-4DCA-BFD8-049948FD6AF9}" name="Svartype" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{F9601F41-BCF3-4490-BF63-46C328B14068}" name="Arkfanetittel" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{5B159670-6FD4-410B-97CA-F479EBDF0EA5}" name="Kommentar" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{B339D8CC-5E13-4DCA-BFD8-049948FD6AF9}" name="Svartype" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F9601F41-BCF3-4490-BF63-46C328B14068}" name="Arkfanetittel" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{5B159670-6FD4-410B-97CA-F479EBDF0EA5}" name="Kommentar" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -908,7 +908,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C29"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
         <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>55</v>
@@ -960,7 +960,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>56</v>
@@ -974,7 +974,7 @@
         <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>44</v>
@@ -988,7 +988,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>51</v>
@@ -1002,7 +1002,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>52</v>
@@ -1016,7 +1016,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>57</v>
@@ -1024,30 +1024,30 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,13 +1058,13 @@
         <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,13 +1075,13 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,10 +1092,10 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,10 +1106,10 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1117,13 +1117,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1134,10 +1134,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1148,10 +1148,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,10 +1162,10 @@
         <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,10 +1176,10 @@
         <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,10 +1190,10 @@
         <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1204,10 +1204,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1218,10 +1218,10 @@
         <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,10 +1232,10 @@
         <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1246,10 +1246,10 @@
         <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1260,10 +1260,10 @@
         <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1274,10 +1274,10 @@
         <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,10 +1288,10 @@
         <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1302,21 +1302,21 @@
         <v>42</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>46</v>
@@ -1330,7 +1330,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>47</v>
@@ -1366,82 +1366,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1449,7 +1449,7 @@
         <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1465,112 +1465,112 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>